<commit_message>
Added graphics for decisions trees of crabs and noshows
</commit_message>
<xml_diff>
--- a/crabs/decision-trees-data/crabs-graphics_DTs.xlsx
+++ b/crabs/decision-trees-data/crabs-graphics_DTs.xlsx
@@ -5,19 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmorvalho/Dropbox/1ºSemestre/SAD/Project/SAD_P2/crabs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmorvalho/Dropbox/1ºSemestre/SAD/Project/SAD_P2/crabs/decision-trees-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="min_num_leaf" sheetId="1" r:id="rId1"/>
     <sheet name="min_sample_node" sheetId="2" r:id="rId2"/>
     <sheet name="min_samples_nodes_leaf" sheetId="3" r:id="rId3"/>
+    <sheet name="accuracy-size" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'accuracy-size'!$A$1:$B$4999</definedName>
+    <definedName name="dt_size_1" localSheetId="3">'accuracy-size'!$A$1:$B$4999</definedName>
+    <definedName name="dt_size_2" localSheetId="3">'accuracy-size'!$A$1:$B$99</definedName>
     <definedName name="min_leaf_1" localSheetId="0">min_num_leaf!$A$1:$B$40</definedName>
+    <definedName name="min_nodes" localSheetId="0">min_num_leaf!$C$1:$D$49</definedName>
     <definedName name="min_nodes" localSheetId="1">min_sample_node!$A$1:$B$49</definedName>
     <definedName name="min_nodes_leaf_1" localSheetId="2">min_samples_nodes_leaf!$A$2:$AD$11</definedName>
   </definedNames>
@@ -35,7 +40,23 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="min_leaf" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="1" name="dt_size" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/pmorvalho/Dropbox/1ºSemestre/SAD/Project/SAD_P2/crabs/dt_size.csv" decimal="," thousands=" ">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="dt_size1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/pmorvalho/Dropbox/1ºSemestre/SAD/Project/SAD_P2/noshows/dt_size.csv" decimal="," thousands=" ">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="min_leaf" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/pmorvalho/Dropbox/1ºSemestre/SAD/Project/SAD_P2/crabs/min_leaf.csv" decimal="," thousands=" ">
       <textFields count="2">
         <textField/>
@@ -43,7 +64,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="min_nodes" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="4" name="min_nodes" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/pmorvalho/Dropbox/1ºSemestre/SAD/Project/SAD_P2/crabs/min_nodes.csv" decimal="," thousands=" ">
       <textFields count="2">
         <textField/>
@@ -51,7 +72,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="min_nodes_leaf" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="5" name="min_nodes_leaf" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/pmorvalho/Dropbox/1ºSemestre/SAD/Project/SAD_P2/crabs/min_nodes_leaf.csv" decimal="," thousands=" ">
       <textFields count="30">
         <textField/>
@@ -82,6 +103,14 @@
         <textField/>
         <textField/>
         <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="min_nodes1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/pmorvalho/Dropbox/1ºSemestre/SAD/Project/SAD_P2/crabs/min_nodes.csv" decimal="," thousands=" ">
+      <textFields count="2">
         <textField/>
         <textField/>
       </textFields>
@@ -171,8 +200,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>min_samples_leaf</a:t>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Minimum Samples</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -503,6 +532,350 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>min_samples_nodes</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>min_num_leaf!$C:$C</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>min_num_leaf!$D:$D</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.816666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.816666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.766666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.766666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.833333333333</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.766666666667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.683333333333</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.766666666667</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.766666666667</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.716666666667</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.716666666667</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.716666666667</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.716666666667</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.716666666667</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -511,11 +884,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1602181200"/>
-        <c:axId val="1475456640"/>
+        <c:axId val="789249312"/>
+        <c:axId val="796126064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1602181200"/>
+        <c:axId val="789249312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -556,11 +929,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>min_samples leaf</a:t>
+                  <a:t>Minimum</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> </a:t>
+                  <a:t> Samples</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -632,15 +1005,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1475456640"/>
+        <c:crossAx val="796126064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1475456640"/>
+        <c:axId val="796126064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.6"/>
+          <c:max val="1.0"/>
+          <c:min val="0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -679,7 +1053,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>precision</a:t>
+                  <a:t>Accuracy</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -751,7 +1125,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1602181200"/>
+        <c:crossAx val="789249312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -763,6 +1137,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -815,7 +1221,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1203,11 +1608,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1593927472"/>
-        <c:axId val="1594398112"/>
+        <c:axId val="789259328"/>
+        <c:axId val="789262448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1593927472"/>
+        <c:axId val="789259328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1257,7 +1662,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1323,12 +1727,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1594398112"/>
+        <c:crossAx val="789262448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1594398112"/>
+        <c:axId val="789262448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.6"/>
@@ -1375,7 +1779,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1442,7 +1845,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1593927472"/>
+        <c:crossAx val="789259328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1525,14 +1928,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>min_samples</a:t>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Minimum samples</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> nodes vs leafs</a:t>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> in nodes with mininimum samples in leafs</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2035,11 +2438,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1488747952"/>
-        <c:axId val="1488751856"/>
+        <c:axId val="789293696"/>
+        <c:axId val="796063456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1488747952"/>
+        <c:axId val="789293696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2080,7 +2483,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>min_samples_leaf</a:t>
+                  <a:t>Minimum Samples in Leafs</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2152,15 +2555,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1488751856"/>
+        <c:crossAx val="796063456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1488751856"/>
+        <c:axId val="796063456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.6"/>
+          <c:max val="1.0"/>
+          <c:min val="0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2199,7 +2603,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>accuracy</a:t>
+                  <a:t>Accuracy</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2270,7 +2674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1488747952"/>
+        <c:crossAx val="789293696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2314,6 +2718,1027 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Size of Tree</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>size</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'accuracy-size'!$A:$A</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>35.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'accuracy-size'!$B:$B</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.716666666667</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.716666666667</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.716666666667</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.716666666667</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.716666666667</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.716666666667</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.766666666667</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.766666666667</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.766666666667</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.716666666667</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.833333333333</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.816666666667</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.766666666667</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.733333333333</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.783333333333</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="789328992"/>
+        <c:axId val="789332752"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="789328992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Size of tree </a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>(number of nodes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="789332752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="789332752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Accuracy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="789328992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2471,6 +3896,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3504,6 +4969,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4124,16 +6105,63 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133864</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>91531</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>652162</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>158807</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="min_leaf_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="min_leaf_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="min_nodes" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="min_nodes" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="min_nodes_leaf_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="min_nodes" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="min_nodes_leaf_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dt_size_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dt_size_2" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4399,10 +6427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4413,324 +6441,636 @@
     <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
         <v>0.83333333333299997</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3">
         <v>0.86666666666699999</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>0.81666666666700005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
         <v>0.78333333333300004</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5">
         <v>0.76666666666700001</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>0.81666666666700005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6">
         <v>0.73333333333299999</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>0.76666666666700001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7">
         <v>0.68333333333299995</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>0.76666666666700001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>0.83333333333299997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
       <c r="B11">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>0.76666666666700001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>12</v>
       </c>
       <c r="B12">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>0.68333333333299995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>15</v>
       </c>
       <c r="B15">
         <v>0.73333333333299999</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16">
         <v>0.78333333333300004</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>17</v>
+      </c>
+      <c r="D16">
+        <v>0.76666666666700001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>17</v>
       </c>
       <c r="B17">
         <v>0.78333333333300004</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>18</v>
+      </c>
+      <c r="D17">
+        <v>0.76666666666700001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>18</v>
       </c>
       <c r="B18">
         <v>0.78333333333300004</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>19</v>
+      </c>
+      <c r="D18">
+        <v>0.71666666666699996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>19</v>
       </c>
       <c r="B19">
         <v>0.73333333333299999</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20</v>
       </c>
       <c r="B20">
         <v>0.78333333333300004</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>21</v>
+      </c>
+      <c r="D20">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>21</v>
       </c>
       <c r="B21">
         <v>0.73333333333299999</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>22</v>
+      </c>
+      <c r="D21">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>22</v>
       </c>
       <c r="B22">
         <v>0.73333333333299999</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>23</v>
+      </c>
+      <c r="D22">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>23</v>
       </c>
       <c r="B23">
         <v>0.76666666666700001</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>24</v>
+      </c>
+      <c r="D23">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>24</v>
       </c>
       <c r="B24">
         <v>0.76666666666700001</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>25</v>
+      </c>
+      <c r="D24">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>25</v>
       </c>
       <c r="B25">
         <v>0.81666666666700005</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>26</v>
+      </c>
+      <c r="D25">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>26</v>
       </c>
       <c r="B26">
         <v>0.81666666666700005</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <v>27</v>
+      </c>
+      <c r="D26">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>27</v>
       </c>
       <c r="B27">
         <v>0.76666666666700001</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>28</v>
+      </c>
+      <c r="D27">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>28</v>
       </c>
       <c r="B28">
         <v>0.83333333333299997</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>29</v>
+      </c>
+      <c r="D28">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>29</v>
       </c>
       <c r="B29">
         <v>0.81666666666700005</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>30</v>
+      </c>
+      <c r="D29">
+        <v>0.71666666666699996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>30</v>
       </c>
       <c r="B30">
         <v>0.81666666666700005</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>31</v>
+      </c>
+      <c r="D30">
+        <v>0.71666666666699996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>31</v>
       </c>
       <c r="B31">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <v>32</v>
+      </c>
+      <c r="D31">
+        <v>0.71666666666699996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>32</v>
       </c>
       <c r="B32">
         <v>0.66666666666700003</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>33</v>
+      </c>
+      <c r="D32">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>33</v>
       </c>
       <c r="B33">
         <v>0.66666666666700003</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>34</v>
+      </c>
+      <c r="D33">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>34</v>
       </c>
       <c r="B34">
         <v>0.66666666666700003</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>35</v>
+      </c>
+      <c r="D34">
+        <v>0.71666666666699996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>35</v>
       </c>
       <c r="B35">
         <v>0.66666666666700003</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>36</v>
+      </c>
+      <c r="D35">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>36</v>
       </c>
       <c r="B36">
         <v>0.66666666666700003</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>37</v>
+      </c>
+      <c r="D36">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>37</v>
       </c>
       <c r="B37">
         <v>0.66666666666700003</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <v>38</v>
+      </c>
+      <c r="D37">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>38</v>
       </c>
       <c r="B38">
         <v>0.66666666666700003</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <v>39</v>
+      </c>
+      <c r="D38">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>39</v>
       </c>
       <c r="B39">
         <v>0.66666666666700003</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <v>40</v>
+      </c>
+      <c r="D39">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>40</v>
       </c>
       <c r="B40">
         <v>0.66666666666700003</v>
+      </c>
+      <c r="C40">
+        <v>41</v>
+      </c>
+      <c r="D40">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>42</v>
+      </c>
+      <c r="D41">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <v>43</v>
+      </c>
+      <c r="D42">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <v>44</v>
+      </c>
+      <c r="D43">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <v>45</v>
+      </c>
+      <c r="D44">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <v>46</v>
+      </c>
+      <c r="D45">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <v>47</v>
+      </c>
+      <c r="D46">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <v>48</v>
+      </c>
+      <c r="D47">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <v>49</v>
+      </c>
+      <c r="D48">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <v>50</v>
+      </c>
+      <c r="D49">
+        <v>0.78333333333300004</v>
       </c>
     </row>
   </sheetData>
@@ -4744,7 +7084,7 @@
   <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection sqref="A1:B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5155,7 +7495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X11"/>
   <sheetViews>
-    <sheetView topLeftCell="C11" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="E7" zoomScale="125" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -5541,4 +7881,823 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B99"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>3</v>
+      </c>
+      <c r="B1">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>7</v>
+      </c>
+      <c r="B37">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>7</v>
+      </c>
+      <c r="B39">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>7</v>
+      </c>
+      <c r="B40">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="B41">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="B42">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>7</v>
+      </c>
+      <c r="B44">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>7</v>
+      </c>
+      <c r="B45">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>7</v>
+      </c>
+      <c r="B46">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>7</v>
+      </c>
+      <c r="B48">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>7</v>
+      </c>
+      <c r="B49">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>7</v>
+      </c>
+      <c r="B50">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>7</v>
+      </c>
+      <c r="B51">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>7</v>
+      </c>
+      <c r="B52">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>7</v>
+      </c>
+      <c r="B53">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>7</v>
+      </c>
+      <c r="B54">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>7</v>
+      </c>
+      <c r="B55">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>9</v>
+      </c>
+      <c r="B56">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>9</v>
+      </c>
+      <c r="B57">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>9</v>
+      </c>
+      <c r="B58">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>11</v>
+      </c>
+      <c r="B59">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>11</v>
+      </c>
+      <c r="B60">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>11</v>
+      </c>
+      <c r="B61">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>11</v>
+      </c>
+      <c r="B62">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>11</v>
+      </c>
+      <c r="B63">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>11</v>
+      </c>
+      <c r="B64">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>11</v>
+      </c>
+      <c r="B65">
+        <v>0.71666666666699996</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>11</v>
+      </c>
+      <c r="B66">
+        <v>0.71666666666699996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>11</v>
+      </c>
+      <c r="B67">
+        <v>0.71666666666699996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>13</v>
+      </c>
+      <c r="B68">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>13</v>
+      </c>
+      <c r="B69">
+        <v>0.66666666666700003</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>13</v>
+      </c>
+      <c r="B70">
+        <v>0.71666666666699996</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>13</v>
+      </c>
+      <c r="B71">
+        <v>0.71666666666699996</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>13</v>
+      </c>
+      <c r="B72">
+        <v>0.71666666666699996</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>17</v>
+      </c>
+      <c r="B73">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>17</v>
+      </c>
+      <c r="B74">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>17</v>
+      </c>
+      <c r="B75">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>17</v>
+      </c>
+      <c r="B76">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>17</v>
+      </c>
+      <c r="B77">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>17</v>
+      </c>
+      <c r="B78">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>17</v>
+      </c>
+      <c r="B79">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>19</v>
+      </c>
+      <c r="B80">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>19</v>
+      </c>
+      <c r="B81">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>19</v>
+      </c>
+      <c r="B82">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>21</v>
+      </c>
+      <c r="B83">
+        <v>0.76666666666700001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>21</v>
+      </c>
+      <c r="B84">
+        <v>0.76666666666700001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>21</v>
+      </c>
+      <c r="B85">
+        <v>0.76666666666700001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>21</v>
+      </c>
+      <c r="B86">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>21</v>
+      </c>
+      <c r="B87">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>23</v>
+      </c>
+      <c r="B88">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>23</v>
+      </c>
+      <c r="B89">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>25</v>
+      </c>
+      <c r="B90">
+        <v>0.71666666666699996</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>27</v>
+      </c>
+      <c r="B91">
+        <v>0.83333333333299997</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>29</v>
+      </c>
+      <c r="B92">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>29</v>
+      </c>
+      <c r="B93">
+        <v>0.81666666666700005</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>29</v>
+      </c>
+      <c r="B94">
+        <v>0.76666666666700001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>31</v>
+      </c>
+      <c r="B95">
+        <v>0.73333333333299999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>33</v>
+      </c>
+      <c r="B96">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>33</v>
+      </c>
+      <c r="B97">
+        <v>0.78333333333300004</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>33</v>
+      </c>
+      <c r="B98">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>35</v>
+      </c>
+      <c r="B99">
+        <v>0.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B4999">
+    <sortState ref="A2:B4999">
+      <sortCondition ref="A1:A4999"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>